<commit_message>
Forms of reports have been adjusted according to the requirement of the customer.
</commit_message>
<xml_diff>
--- a/Reports/Отчет - ТипыПроектов.xlsx
+++ b/Reports/Отчет - ТипыПроектов.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24827"/>
   <workbookPr filterPrivacy="1" codeName="ЭтаКнига"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{84B63E7E-8610-40A4-9E7F-990F68B6C813}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B6DADCB6-8485-49C8-AAC3-436D3E1E1AB5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-28920" yWindow="-12045" windowWidth="29040" windowHeight="17640" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -909,6 +909,14 @@
     <xf numFmtId="0" fontId="10" fillId="0" borderId="6" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="20" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="20" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="26" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -921,10 +929,6 @@
     <xf numFmtId="0" fontId="10" fillId="2" borderId="27" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="20" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="6" borderId="24" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -934,10 +938,6 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="20" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Обычный" xfId="0" builtinId="0"/>
@@ -1290,7 +1290,7 @@
     <col min="1" max="1" width="2.7109375" style="1" customWidth="1"/>
     <col min="2" max="2" width="14" style="1" customWidth="1"/>
     <col min="3" max="3" width="9.28515625" style="1" customWidth="1"/>
-    <col min="4" max="4" width="16" style="1" customWidth="1"/>
+    <col min="4" max="4" width="18.85546875" style="1" customWidth="1"/>
     <col min="5" max="5" width="6.7109375" style="1" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="6.42578125" style="1" customWidth="1"/>
     <col min="7" max="7" width="6.5703125" style="1" bestFit="1" customWidth="1"/>
@@ -1558,13 +1558,13 @@
         <v>1</v>
       </c>
       <c r="D4" s="22" t="s">
-        <v>69</v>
-      </c>
-      <c r="E4" s="40" t="str">
+        <v>73</v>
+      </c>
+      <c r="E4" s="42" t="str">
         <f>VLOOKUP(УникальныеСписки!A1,Настройки!A1:D50,4,FALSE)</f>
         <v>AB</v>
       </c>
-      <c r="F4" s="41"/>
+      <c r="F4" s="43"/>
       <c r="G4" s="23">
         <f>ROW(B9)-2</f>
         <v>7</v>
@@ -1575,41 +1575,41 @@
         <f>""</f>
         <v/>
       </c>
-      <c r="B5" s="42" t="s">
+      <c r="B5" s="44" t="s">
         <v>3</v>
       </c>
-      <c r="C5" s="36" t="s">
+      <c r="C5" s="40" t="s">
         <v>57</v>
       </c>
-      <c r="D5" s="34" t="s">
+      <c r="D5" s="38" t="s">
         <v>68</v>
       </c>
-      <c r="E5" s="45" t="s">
+      <c r="E5" s="36" t="s">
         <v>59</v>
       </c>
-      <c r="F5" s="46"/>
-      <c r="G5" s="46"/>
-      <c r="H5" s="46"/>
-      <c r="I5" s="46"/>
-      <c r="J5" s="46"/>
-      <c r="K5" s="46"/>
-      <c r="L5" s="46"/>
-      <c r="M5" s="46"/>
-      <c r="N5" s="46"/>
-      <c r="O5" s="46"/>
-      <c r="P5" s="46"/>
-      <c r="Q5" s="46"/>
-      <c r="R5" s="46"/>
-      <c r="S5" s="46"/>
-      <c r="T5" s="46"/>
-      <c r="U5" s="46"/>
-      <c r="V5" s="46"/>
-      <c r="W5" s="46"/>
-      <c r="X5" s="46"/>
-      <c r="Y5" s="46"/>
-      <c r="Z5" s="46"/>
-      <c r="AA5" s="46"/>
-      <c r="AB5" s="39"/>
+      <c r="F5" s="37"/>
+      <c r="G5" s="37"/>
+      <c r="H5" s="37"/>
+      <c r="I5" s="37"/>
+      <c r="J5" s="37"/>
+      <c r="K5" s="37"/>
+      <c r="L5" s="37"/>
+      <c r="M5" s="37"/>
+      <c r="N5" s="37"/>
+      <c r="O5" s="37"/>
+      <c r="P5" s="37"/>
+      <c r="Q5" s="37"/>
+      <c r="R5" s="37"/>
+      <c r="S5" s="37"/>
+      <c r="T5" s="37"/>
+      <c r="U5" s="37"/>
+      <c r="V5" s="37"/>
+      <c r="W5" s="37"/>
+      <c r="X5" s="37"/>
+      <c r="Y5" s="37"/>
+      <c r="Z5" s="37"/>
+      <c r="AA5" s="37"/>
+      <c r="AB5" s="35"/>
       <c r="AC5" s="4"/>
     </row>
     <row r="6" spans="1:29" ht="9.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -1617,57 +1617,57 @@
         <f>""</f>
         <v/>
       </c>
-      <c r="B6" s="43"/>
-      <c r="C6" s="37"/>
-      <c r="D6" s="35"/>
-      <c r="E6" s="38" t="s">
+      <c r="B6" s="45"/>
+      <c r="C6" s="41"/>
+      <c r="D6" s="39"/>
+      <c r="E6" s="34" t="s">
         <v>5</v>
       </c>
-      <c r="F6" s="39"/>
-      <c r="G6" s="38" t="s">
+      <c r="F6" s="35"/>
+      <c r="G6" s="34" t="s">
         <v>6</v>
       </c>
-      <c r="H6" s="39"/>
-      <c r="I6" s="38" t="s">
+      <c r="H6" s="35"/>
+      <c r="I6" s="34" t="s">
         <v>7</v>
       </c>
-      <c r="J6" s="39"/>
-      <c r="K6" s="38" t="s">
+      <c r="J6" s="35"/>
+      <c r="K6" s="34" t="s">
         <v>8</v>
       </c>
-      <c r="L6" s="39"/>
-      <c r="M6" s="38" t="s">
+      <c r="L6" s="35"/>
+      <c r="M6" s="34" t="s">
         <v>9</v>
       </c>
-      <c r="N6" s="39"/>
-      <c r="O6" s="38" t="s">
+      <c r="N6" s="35"/>
+      <c r="O6" s="34" t="s">
         <v>10</v>
       </c>
-      <c r="P6" s="39"/>
-      <c r="Q6" s="38" t="s">
+      <c r="P6" s="35"/>
+      <c r="Q6" s="34" t="s">
         <v>11</v>
       </c>
-      <c r="R6" s="39"/>
-      <c r="S6" s="38" t="s">
+      <c r="R6" s="35"/>
+      <c r="S6" s="34" t="s">
         <v>12</v>
       </c>
-      <c r="T6" s="39"/>
-      <c r="U6" s="38" t="s">
+      <c r="T6" s="35"/>
+      <c r="U6" s="34" t="s">
         <v>13</v>
       </c>
-      <c r="V6" s="39"/>
-      <c r="W6" s="38" t="s">
+      <c r="V6" s="35"/>
+      <c r="W6" s="34" t="s">
         <v>14</v>
       </c>
-      <c r="X6" s="39"/>
-      <c r="Y6" s="38" t="s">
+      <c r="X6" s="35"/>
+      <c r="Y6" s="34" t="s">
         <v>15</v>
       </c>
-      <c r="Z6" s="39"/>
-      <c r="AA6" s="38" t="s">
+      <c r="Z6" s="35"/>
+      <c r="AA6" s="34" t="s">
         <v>16</v>
       </c>
-      <c r="AB6" s="39"/>
+      <c r="AB6" s="35"/>
       <c r="AC6" s="4"/>
     </row>
     <row r="7" spans="1:29" ht="9.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -1675,9 +1675,9 @@
         <f>""</f>
         <v/>
       </c>
-      <c r="B7" s="43"/>
-      <c r="C7" s="37"/>
-      <c r="D7" s="35"/>
+      <c r="B7" s="45"/>
+      <c r="C7" s="41"/>
+      <c r="D7" s="39"/>
       <c r="E7" s="11" t="s">
         <v>17</v>
       </c>
@@ -1757,7 +1757,7 @@
         <f>""</f>
         <v/>
       </c>
-      <c r="B8" s="44"/>
+      <c r="B8" s="46"/>
       <c r="C8" s="31"/>
       <c r="D8" s="31"/>
       <c r="E8" s="8"/>
@@ -6651,6 +6651,11 @@
   </sheetData>
   <autoFilter ref="C8:AB50" xr:uid="{00000000-0009-0000-0000-000000000000}"/>
   <mergeCells count="17">
+    <mergeCell ref="D5:D7"/>
+    <mergeCell ref="C5:C7"/>
+    <mergeCell ref="K6:L6"/>
+    <mergeCell ref="E4:F4"/>
+    <mergeCell ref="B5:B8"/>
     <mergeCell ref="W6:X6"/>
     <mergeCell ref="E5:AB5"/>
     <mergeCell ref="M6:N6"/>
@@ -6663,11 +6668,6 @@
     <mergeCell ref="S6:T6"/>
     <mergeCell ref="U6:V6"/>
     <mergeCell ref="Y6:Z6"/>
-    <mergeCell ref="D5:D7"/>
-    <mergeCell ref="C5:C7"/>
-    <mergeCell ref="K6:L6"/>
-    <mergeCell ref="E4:F4"/>
-    <mergeCell ref="B5:B8"/>
   </mergeCells>
   <conditionalFormatting sqref="E2:AB2">
     <cfRule type="expression" dxfId="2" priority="6">

</xml_diff>